<commit_message>
fix in river levels and adjusted regional gradient
</commit_message>
<xml_diff>
--- a/data/par.xlsx
+++ b/data/par.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apryet/recherche/rezin/drainage/model_sescousse/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF47B53-7A4C-C64B-B670-64CAFC9890BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD334D5-DE45-E64F-980E-5459F5176528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7980" yWindow="560" windowWidth="20820" windowHeight="17440" xr2:uid="{B057D5EE-0016-6343-8953-8CB9525BC8FD}"/>
+    <workbookView xWindow="700" yWindow="500" windowWidth="27400" windowHeight="17500" xr2:uid="{B057D5EE-0016-6343-8953-8CB9525BC8FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -114,7 +114,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -129,13 +129,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -150,10 +164,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,40 +486,40 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -518,19 +533,19 @@
       <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>1E-3</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>0.01</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <v>1E-8</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="1">
         <v>1</v>
       </c>
     </row>
@@ -570,20 +585,20 @@
       <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <f>$D$2*40</f>
         <v>0.04</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>1E-4</v>
       </c>
       <c r="F4">
         <v>100</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>1E-8</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>100</v>
       </c>
     </row>
@@ -597,20 +612,20 @@
       <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <f>$D$2*40</f>
         <v>0.04</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>1E-4</v>
       </c>
       <c r="F5">
         <v>100</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>1E-8</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>100</v>
       </c>
     </row>
@@ -624,19 +639,19 @@
       <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="2">
-        <v>17.600000000000001</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="D6" s="1">
+        <v>18.7</v>
+      </c>
+      <c r="E6" s="1">
         <v>15</v>
       </c>
       <c r="F6">
         <v>20</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>1E-8</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1">
         <v>100</v>
       </c>
     </row>
@@ -650,19 +665,19 @@
       <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="2">
-        <v>22.21</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="D7" s="1">
+        <v>20.91</v>
+      </c>
+      <c r="E7" s="1">
         <v>20</v>
       </c>
       <c r="F7">
         <v>25</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>1E-8</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1">
         <v>100</v>
       </c>
     </row>
@@ -676,19 +691,19 @@
       <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>1E-4</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>1E-4</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <v>1E-8</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="1">
         <v>100</v>
       </c>
     </row>
@@ -702,19 +717,19 @@
       <c r="C9" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>1E-3</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <v>1E-8</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1">
         <v>100</v>
       </c>
     </row>
@@ -728,19 +743,19 @@
       <c r="C10" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>0.2</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>0.05</v>
       </c>
       <c r="F10">
         <v>0.8</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
         <v>1E-3</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="1">
         <v>1</v>
       </c>
     </row>
@@ -754,19 +769,19 @@
       <c r="C11" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>25</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>2.5</v>
       </c>
       <c r="F11">
         <v>100</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
         <v>1</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="1">
         <v>1000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
edits and sim dir
</commit_message>
<xml_diff>
--- a/data/par.xlsx
+++ b/data/par.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apryet/recherche/rezin/drainage/model_sescousse/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD334D5-DE45-E64F-980E-5459F5176528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581B9F96-7EA7-4640-A4DF-B7B301C97EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="500" windowWidth="27400" windowHeight="17500" xr2:uid="{B057D5EE-0016-6343-8953-8CB9525BC8FD}"/>
+    <workbookView xWindow="1320" yWindow="760" windowWidth="24300" windowHeight="14120" xr2:uid="{B057D5EE-0016-6343-8953-8CB9525BC8FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -485,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C5A993-0474-574E-A705-662DE965F119}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -537,7 +537,7 @@
         <v>1E-3</v>
       </c>
       <c r="E2" s="1">
-        <v>9.9999999999999995E-7</v>
+        <v>1E-4</v>
       </c>
       <c r="F2" s="1">
         <v>0.01</v>
@@ -563,7 +563,7 @@
         <v>0.1</v>
       </c>
       <c r="E3">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="F3">
         <v>0.5</v>
@@ -586,14 +586,13 @@
         <v>16</v>
       </c>
       <c r="D4" s="1">
-        <f>$D$2*40</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E4" s="1">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="F4">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1">
         <v>1E-8</v>
@@ -613,14 +612,13 @@
         <v>16</v>
       </c>
       <c r="D5" s="1">
-        <f>$D$2*40</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E5" s="1">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="F5">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1">
         <v>1E-8</v>
@@ -695,10 +693,10 @@
         <v>1E-4</v>
       </c>
       <c r="E8" s="1">
-        <v>1E-4</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="G8" s="1">
         <v>1E-8</v>
@@ -721,10 +719,10 @@
         <v>1E-3</v>
       </c>
       <c r="E9" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>1E-4</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="G9" s="1">
         <v>1E-8</v>
@@ -744,13 +742,14 @@
         <v>16</v>
       </c>
       <c r="D10" s="1">
-        <v>0.2</v>
+        <f>10^((LOG10(E10)+LOG10(F10))/2)</f>
+        <v>0.15811388300841889</v>
       </c>
       <c r="E10" s="1">
         <v>0.05</v>
       </c>
       <c r="F10">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="G10" s="1">
         <v>1E-3</v>
@@ -770,13 +769,14 @@
         <v>16</v>
       </c>
       <c r="D11" s="1">
-        <v>25</v>
+        <f>10^((LOG10(E11)+LOG10(F11))/2)</f>
+        <v>11.180339887498951</v>
       </c>
       <c r="E11" s="1">
         <v>2.5</v>
       </c>
       <c r="F11">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G11" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
revised obs. ref, river slope, extended cal period, fixed rbot
</commit_message>
<xml_diff>
--- a/data/par.xlsx
+++ b/data/par.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apryet/recherche/rezin/drainage/model_sescousse/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581B9F96-7EA7-4640-A4DF-B7B301C97EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4AD672-A66A-844A-A0C7-CFCBB9D65BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="760" windowWidth="24300" windowHeight="14120" xr2:uid="{B057D5EE-0016-6343-8953-8CB9525BC8FD}"/>
+    <workbookView xWindow="5180" yWindow="1180" windowWidth="29060" windowHeight="15820" xr2:uid="{B057D5EE-0016-6343-8953-8CB9525BC8FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t>name</t>
   </si>
@@ -95,19 +95,25 @@
     <t>cghbe</t>
   </si>
   <si>
-    <t>hghbw</t>
-  </si>
-  <si>
-    <t>hghbe</t>
-  </si>
-  <si>
-    <t>hghb</t>
-  </si>
-  <si>
-    <t>fixed</t>
-  </si>
-  <si>
     <t>pargp</t>
+  </si>
+  <si>
+    <t>kc</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>dhghbw</t>
+  </si>
+  <si>
+    <t>dhghbe</t>
+  </si>
+  <si>
+    <t>dhriv</t>
+  </si>
+  <si>
+    <t>dh</t>
   </si>
 </sst>
 </file>
@@ -483,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C5A993-0474-574E-A705-662DE965F119}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -496,7 +502,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
@@ -629,97 +635,97 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
       <c r="D6" s="1">
-        <v>18.7</v>
+        <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>15</v>
+        <v>-0.25</v>
       </c>
       <c r="F6">
-        <v>20</v>
+        <v>0.25</v>
       </c>
       <c r="G6" s="1">
-        <v>1E-8</v>
+        <v>-10</v>
       </c>
       <c r="H6" s="1">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
       <c r="D7" s="1">
-        <v>20.91</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1">
-        <v>20</v>
+        <v>-0.25</v>
       </c>
       <c r="F7">
-        <v>25</v>
+        <v>0.25</v>
       </c>
       <c r="G7" s="1">
-        <v>1E-8</v>
+        <v>-10</v>
       </c>
       <c r="H7" s="1">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="E8" s="1">
-        <v>9.9999999999999995E-7</v>
+        <v>-0.25</v>
       </c>
       <c r="F8">
-        <v>0.01</v>
+        <v>0.25</v>
       </c>
       <c r="G8" s="1">
-        <v>1E-8</v>
+        <v>-10</v>
       </c>
       <c r="H8" s="1">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="1">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="E9" s="1">
-        <v>1E-4</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="F9">
         <v>0.01</v>
@@ -733,56 +739,108 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="1">
-        <f>10^((LOG10(E10)+LOG10(F10))/2)</f>
-        <v>0.15811388300841889</v>
+        <v>1E-3</v>
       </c>
       <c r="E10" s="1">
-        <v>0.05</v>
+        <v>1E-4</v>
       </c>
       <c r="F10">
-        <v>0.5</v>
+        <v>0.01</v>
       </c>
       <c r="G10" s="1">
-        <v>1E-3</v>
+        <v>1E-8</v>
       </c>
       <c r="H10" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="1">
         <f>10^((LOG10(E11)+LOG10(F11))/2)</f>
-        <v>11.180339887498951</v>
+        <v>7.0710678118654738E-2</v>
       </c>
       <c r="E11" s="1">
-        <v>2.5</v>
+        <v>0.01</v>
       </c>
       <c r="F11">
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="1">
+        <f>10^((LOG10(E12)+LOG10(F12))/2)</f>
+        <v>4.9999999999999991</v>
+      </c>
+      <c r="E12">
+        <v>0.5</v>
+      </c>
+      <c r="F12">
         <v>50</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G12" s="1">
         <v>1</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H12" s="1">
         <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>